<commit_message>
Updating the code add features such as deleting Cards and more information to cards like Industry
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b8365288089222e/Code/PythonProjects/FlaskCRMTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_F25DC773A252ABDACC1048FD99DF72805BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28BAC80A-FF7D-43E0-A7FA-B37FFAF17B11}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="11_F25DC773A252ABDACC1048FD99DF72805BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D7EE880-E6DE-441D-9E99-38BFAA4F002D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="2850" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -151,13 +151,49 @@
   </si>
   <si>
     <t>Last_Meeting</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Supply Chain</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Ecommerce</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Banking</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,12 +208,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,7 +241,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,10 +542,10 @@
     <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -545,10 +574,13 @@
         <v>41</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -567,17 +599,20 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4">
-        <v>1735689600</v>
+      <c r="H2" s="2">
+        <v>45658</v>
       </c>
       <c r="I2" s="2">
         <v>45658</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -596,17 +631,20 @@
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="4">
-        <v>1735689600</v>
+      <c r="H3" s="2">
+        <v>45658</v>
       </c>
       <c r="I3" s="2">
         <v>45658</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -625,17 +663,20 @@
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="4">
-        <v>1735689600</v>
+      <c r="H4" s="2">
+        <v>45658</v>
       </c>
       <c r="I4" s="2">
         <v>45658</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -654,17 +695,20 @@
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="4">
-        <v>1735689600</v>
+      <c r="H5" s="2">
+        <v>45658</v>
       </c>
       <c r="I5" s="2">
         <v>45658</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -683,17 +727,20 @@
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="4">
-        <v>1735689600</v>
+      <c r="H6" s="2">
+        <v>45658</v>
       </c>
       <c r="I6" s="2">
         <v>45658</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -712,17 +759,20 @@
       <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4">
-        <v>1735689600</v>
+      <c r="H7" s="2">
+        <v>45658</v>
       </c>
       <c r="I7" s="2">
         <v>45658</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -741,17 +791,20 @@
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="4">
-        <v>1735689600</v>
+      <c r="H8" s="2">
+        <v>45658</v>
       </c>
       <c r="I8" s="2">
         <v>45658</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -770,17 +823,20 @@
       <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="4">
-        <v>1735689600</v>
+      <c r="H9" s="2">
+        <v>45658</v>
       </c>
       <c r="I9" s="2">
         <v>45658</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -799,17 +855,20 @@
       <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="4">
-        <v>1735689600</v>
+      <c r="H10" s="2">
+        <v>45658</v>
       </c>
       <c r="I10" s="2">
         <v>45658</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -828,17 +887,20 @@
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="4">
-        <v>1735689600</v>
+      <c r="H11" s="2">
+        <v>45658</v>
       </c>
       <c r="I11" s="2">
         <v>45658</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -857,17 +919,20 @@
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="4">
-        <v>1735689600</v>
+      <c r="H12" s="2">
+        <v>45658</v>
       </c>
       <c r="I12" s="2">
         <v>45658</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -886,17 +951,20 @@
       <c r="F13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="4">
-        <v>1735689600</v>
+      <c r="H13" s="2">
+        <v>45658</v>
       </c>
       <c r="I13" s="2">
         <v>45658</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -915,17 +983,20 @@
       <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="4">
-        <v>1735689600</v>
+      <c r="H14" s="2">
+        <v>45658</v>
       </c>
       <c r="I14" s="2">
         <v>45658</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -944,17 +1015,20 @@
       <c r="F15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="4">
-        <v>1735689600</v>
+      <c r="H15" s="2">
+        <v>45658</v>
       </c>
       <c r="I15" s="2">
         <v>45658</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -973,17 +1047,20 @@
       <c r="F16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="4">
-        <v>1735689600</v>
+      <c r="H16" s="2">
+        <v>45658</v>
       </c>
       <c r="I16" s="2">
         <v>45658</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1002,17 +1079,20 @@
       <c r="F17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="4">
-        <v>1735689600</v>
+      <c r="H17" s="2">
+        <v>45658</v>
       </c>
       <c r="I17" s="2">
         <v>45658</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1031,17 +1111,20 @@
       <c r="F18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="4">
-        <v>1735689600</v>
+      <c r="H18" s="2">
+        <v>45658</v>
       </c>
       <c r="I18" s="2">
         <v>45658</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1060,13 +1143,16 @@
       <c r="F19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="4">
-        <v>1735689600</v>
+      <c r="H19" s="2">
+        <v>45658</v>
       </c>
       <c r="I19" s="2">
         <v>45658</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made some quick bugfixes
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b8365288089222e/Code/PythonProjects/FlaskCRMTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="11_F25DC773A252ABDACC1048FD99DF72805BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D7EE880-E6DE-441D-9E99-38BFAA4F002D}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="11_F25DC773A252ABDACC1048FD99DF72805BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34461004-62CC-4267-998A-82CDE54B5DA9}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2850" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="6330" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -187,13 +187,70 @@
   </si>
   <si>
     <t>Banking</t>
+  </si>
+  <si>
+    <t>Phone_Number</t>
+  </si>
+  <si>
+    <t>0126906297</t>
+  </si>
+  <si>
+    <t>0126906298</t>
+  </si>
+  <si>
+    <t>0126906299</t>
+  </si>
+  <si>
+    <t>0126906300</t>
+  </si>
+  <si>
+    <t>0126906301</t>
+  </si>
+  <si>
+    <t>0126906302</t>
+  </si>
+  <si>
+    <t>0126906303</t>
+  </si>
+  <si>
+    <t>0126906304</t>
+  </si>
+  <si>
+    <t>0126906305</t>
+  </si>
+  <si>
+    <t>0126906306</t>
+  </si>
+  <si>
+    <t>0126906307</t>
+  </si>
+  <si>
+    <t>0126906308</t>
+  </si>
+  <si>
+    <t>0126906309</t>
+  </si>
+  <si>
+    <t>0126906310</t>
+  </si>
+  <si>
+    <t>0126906311</t>
+  </si>
+  <si>
+    <t>0126906312</t>
+  </si>
+  <si>
+    <t>0126906313</t>
+  </si>
+  <si>
+    <t>0126906314</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +262,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +302,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -525,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,16 +605,17 @@
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="17" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -555,32 +625,35 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -590,29 +663,32 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2">
-        <v>45658</v>
-      </c>
       <c r="I2" s="2">
         <v>45658</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K2" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -622,29 +698,32 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="2">
-        <v>45658</v>
-      </c>
       <c r="I3" s="2">
         <v>45658</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K3" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -654,29 +733,32 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="2">
-        <v>45658</v>
-      </c>
       <c r="I4" s="2">
         <v>45658</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K4" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -686,29 +768,32 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="2">
-        <v>45658</v>
-      </c>
       <c r="I5" s="2">
         <v>45658</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K5" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -718,29 +803,32 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>4</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="2">
-        <v>45658</v>
-      </c>
       <c r="I6" s="2">
         <v>45658</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K6" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -750,29 +838,32 @@
       <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="2">
-        <v>45658</v>
-      </c>
       <c r="I7" s="2">
         <v>45658</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -782,29 +873,32 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="2">
-        <v>45658</v>
-      </c>
       <c r="I8" s="2">
         <v>45658</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K8" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -814,29 +908,32 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="2">
-        <v>45658</v>
-      </c>
       <c r="I9" s="2">
         <v>45658</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K9" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -846,29 +943,32 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="2">
-        <v>45658</v>
-      </c>
       <c r="I10" s="2">
         <v>45658</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K10" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -878,29 +978,32 @@
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="2">
-        <v>45658</v>
-      </c>
       <c r="I11" s="2">
         <v>45658</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K11" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -910,29 +1013,32 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="2">
-        <v>45658</v>
-      </c>
       <c r="I12" s="2">
         <v>45658</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K12" t="s">
         <v>48</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -942,29 +1048,32 @@
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="2">
-        <v>45658</v>
-      </c>
       <c r="I13" s="2">
         <v>45658</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K13" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -974,29 +1083,32 @@
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="2">
-        <v>45658</v>
-      </c>
       <c r="I14" s="2">
         <v>45658</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K14" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1006,29 +1118,32 @@
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>5</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="2">
-        <v>45658</v>
-      </c>
       <c r="I15" s="2">
         <v>45658</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K15" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1038,29 +1153,32 @@
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>5</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="2">
-        <v>45658</v>
-      </c>
       <c r="I16" s="2">
         <v>45658</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K16" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1070,29 +1188,32 @@
       <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>5</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="2">
-        <v>45658</v>
-      </c>
       <c r="I17" s="2">
         <v>45658</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K17" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1102,29 +1223,32 @@
       <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>5</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="2">
-        <v>45658</v>
-      </c>
       <c r="I18" s="2">
         <v>45658</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K18" t="s">
         <v>52</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1134,29 +1258,33 @@
       <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="2">
-        <v>45658</v>
-      </c>
       <c r="I19" s="2">
         <v>45658</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2">
+        <v>45658</v>
+      </c>
+      <c r="K19" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>